<commit_message>
Fixed HS; doesn't require embedded IS now
> I fixed collision handling for hash sort and removed use of insertion
sort at the end to fix errors
> I added some initial test results to the spreadsheet for HS on my
laptop
</commit_message>
<xml_diff>
--- a/Testing/aa_writing_02.xlsx
+++ b/Testing/aa_writing_02.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rebecca\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -105,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -293,7 +288,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -345,7 +340,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -539,38 +534,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="J85" sqref="J85"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="3"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="3"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
     <col min="11" max="11" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="14" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="13" max="14" width="12.6640625" customWidth="1"/>
     <col min="15" max="15" width="12" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,7 +612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -661,7 +656,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -705,7 +700,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -749,7 +744,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -787,7 +782,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -822,7 +817,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -866,7 +861,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -910,7 +905,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -954,7 +949,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -989,7 +984,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1024,7 +1019,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1068,7 +1063,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1112,7 +1107,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1156,7 +1151,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1200,7 +1195,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1244,7 +1239,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1288,7 +1283,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1332,7 +1327,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1376,7 +1371,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1420,7 +1415,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1464,7 +1459,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1508,7 +1503,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1552,7 +1547,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1596,7 +1591,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1640,7 +1635,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1675,7 +1670,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1719,7 +1714,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1763,7 +1758,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1807,7 +1802,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1845,7 +1840,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1880,7 +1875,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1924,7 +1919,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1968,7 +1963,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -2012,7 +2007,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -2047,7 +2042,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -2082,7 +2077,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -2126,7 +2121,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -2170,7 +2165,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -2214,7 +2209,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -2258,7 +2253,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -2302,7 +2297,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2346,7 +2341,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -2390,7 +2385,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -2434,7 +2429,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -2478,7 +2473,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2522,7 +2517,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -2566,7 +2561,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -2610,7 +2605,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -2654,7 +2649,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -2698,7 +2693,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -2733,7 +2728,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -2777,7 +2772,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -2821,7 +2816,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -2865,7 +2860,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -2909,7 +2904,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -2944,7 +2939,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -2988,7 +2983,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -3032,7 +3027,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3076,7 +3071,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -3120,7 +3115,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -3155,7 +3150,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -3199,7 +3194,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -3243,7 +3238,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -3287,7 +3282,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -3331,7 +3326,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -3375,7 +3370,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -3419,7 +3414,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -3463,7 +3458,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -3507,7 +3502,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -3551,7 +3546,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -3595,7 +3590,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -3639,7 +3634,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -3683,7 +3678,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -3727,7 +3722,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -3771,7 +3766,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -3806,7 +3801,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -3859,7 +3854,7 @@
         <v>1.3240000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -3912,7 +3907,7 @@
         <v>144.22</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -3965,7 +3960,7 @@
         <v>12847.933333333334</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15">
       <c r="A80" t="s">
         <v>15</v>
       </c>
@@ -4015,7 +4010,7 @@
         <v>1283240</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15">
       <c r="A81" t="s">
         <v>15</v>
       </c>
@@ -4050,7 +4045,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15">
       <c r="A82" t="s">
         <v>15</v>
       </c>
@@ -4094,7 +4089,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15">
       <c r="A83" t="s">
         <v>15</v>
       </c>
@@ -4138,7 +4133,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15">
       <c r="A84" t="s">
         <v>15</v>
       </c>
@@ -4182,7 +4177,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -4220,7 +4215,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15">
       <c r="A86" t="s">
         <v>15</v>
       </c>
@@ -4255,7 +4250,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15">
       <c r="A87" t="s">
         <v>15</v>
       </c>
@@ -4308,7 +4303,7 @@
         <v>0.17466666666666666</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15">
       <c r="A88" t="s">
         <v>15</v>
       </c>
@@ -4361,7 +4356,7 @@
         <v>2.0833333333333335</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15">
       <c r="A89" t="s">
         <v>15</v>
       </c>
@@ -4414,7 +4409,7 @@
         <v>27.125666666666664</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15">
       <c r="A90" t="s">
         <v>15</v>
       </c>
@@ -4467,7 +4462,7 @@
         <v>301.93866666666668</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15">
       <c r="A91" t="s">
         <v>15</v>
       </c>
@@ -4520,7 +4515,7 @@
         <v>3439.8233333333337</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15">
       <c r="A92" t="s">
         <v>15</v>
       </c>
@@ -4573,7 +4568,7 @@
         <v>0.14533333333333331</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15">
       <c r="A93" t="s">
         <v>15</v>
       </c>
@@ -4626,7 +4621,7 @@
         <v>1.4303333333333335</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15">
       <c r="A94" t="s">
         <v>15</v>
       </c>
@@ -4679,7 +4674,7 @@
         <v>17.204000000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15">
       <c r="A95" t="s">
         <v>15</v>
       </c>
@@ -4732,7 +4727,7 @@
         <v>207.01999999999998</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15">
       <c r="A96" t="s">
         <v>15</v>
       </c>
@@ -4785,7 +4780,7 @@
         <v>2347.7199999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15">
       <c r="A97" t="s">
         <v>15</v>
       </c>
@@ -4803,24 +4798,33 @@
         <f t="shared" ref="E97:E101" si="23">C97 * LOG(C97, 2)</f>
         <v>9965.7842846620879</v>
       </c>
-      <c r="I97" s="3" t="e">
+      <c r="F97">
+        <v>12.726511</v>
+      </c>
+      <c r="G97">
+        <v>15.246131</v>
+      </c>
+      <c r="H97">
+        <v>13.645118999999999</v>
+      </c>
+      <c r="I97" s="3">
         <f t="shared" ref="I97:I101" si="24">AVERAGE(F97:H97)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J97" t="e">
+        <v>13.872587000000001</v>
+      </c>
+      <c r="J97">
         <f t="shared" ref="J97:J101" si="25">AVERAGE(G97:I97)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K97" s="3" t="e">
+        <v>14.254612333333334</v>
+      </c>
+      <c r="K97" s="3">
         <f t="shared" ref="K97:K101" si="26">I97/E97</f>
-        <v>#DIV/0!</v>
+        <v>1.3920216014860673E-3</v>
       </c>
       <c r="O97" s="3" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15">
       <c r="A98" t="s">
         <v>15</v>
       </c>
@@ -4838,24 +4842,33 @@
         <f t="shared" si="23"/>
         <v>132877.1237954945</v>
       </c>
-      <c r="I98" s="3" t="e">
+      <c r="F98">
+        <v>86.402045999999999</v>
+      </c>
+      <c r="G98">
+        <v>90.485462999999996</v>
+      </c>
+      <c r="H98">
+        <v>83.001548999999997</v>
+      </c>
+      <c r="I98" s="3">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J98" t="e">
+        <v>86.629685999999992</v>
+      </c>
+      <c r="J98">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K98" s="3" t="e">
+        <v>86.70556599999999</v>
+      </c>
+      <c r="K98" s="3">
         <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
+        <v>6.5195335002380121E-4</v>
       </c>
       <c r="O98" s="3" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15">
       <c r="A99" t="s">
         <v>15</v>
       </c>
@@ -4873,24 +4886,33 @@
         <f t="shared" si="23"/>
         <v>1660964.0474436812</v>
       </c>
-      <c r="I99" s="3" t="e">
+      <c r="F99">
+        <v>4542.8524809999999</v>
+      </c>
+      <c r="G99">
+        <v>4719.5939600000002</v>
+      </c>
+      <c r="H99">
+        <v>4667.7834579999999</v>
+      </c>
+      <c r="I99" s="3">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J99" t="e">
+        <v>4643.4099663333336</v>
+      </c>
+      <c r="J99">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K99" s="3" t="e">
+        <v>4676.9291281111109</v>
+      </c>
+      <c r="K99" s="3">
         <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
+        <v>2.7956113640628211E-3</v>
       </c>
       <c r="O99" s="3" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -4925,7 +4947,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15">
       <c r="A101" t="s">
         <v>15</v>
       </c>
@@ -4972,15 +4994,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0478F04A-1D41-4EB4-BD33-BB585464C9D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ran some HS tests and updated description
</commit_message>
<xml_diff>
--- a/Testing/aa_writing_02.xlsx
+++ b/Testing/aa_writing_02.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="24">
   <si>
     <t>Computer</t>
   </si>
@@ -160,8 +160,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -199,7 +201,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -215,6 +217,7 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -230,6 +233,7 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -534,7 +538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,16 +546,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O101"/>
+  <dimension ref="A1:O102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="P101" sqref="P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="8.83203125" style="3"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
@@ -3674,7 +3679,7 @@
         <v>7.1576576877931759E-4</v>
       </c>
       <c r="O73" s="3" t="e">
-        <f t="shared" ref="O73:O101" si="14">AVERAGE(L73:N73)</f>
+        <f t="shared" ref="O73:O102" si="14">AVERAGE(L73:N73)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4791,11 +4796,11 @@
         <v>1000</v>
       </c>
       <c r="D97">
-        <f t="shared" ref="D97:D101" si="22">C97^2</f>
+        <f t="shared" ref="D97:D102" si="22">C97^2</f>
         <v>1000000</v>
       </c>
       <c r="E97" s="3">
-        <f t="shared" ref="E97:E101" si="23">C97 * LOG(C97, 2)</f>
+        <f t="shared" ref="E97:E102" si="23">C97 * LOG(C97, 2)</f>
         <v>9965.7842846620879</v>
       </c>
       <c r="F97">
@@ -4808,15 +4813,15 @@
         <v>13.645118999999999</v>
       </c>
       <c r="I97" s="3">
-        <f t="shared" ref="I97:I101" si="24">AVERAGE(F97:H97)</f>
+        <f t="shared" ref="I97:I102" si="24">AVERAGE(F97:H97)</f>
         <v>13.872587000000001</v>
       </c>
       <c r="J97">
-        <f t="shared" ref="J97:J101" si="25">AVERAGE(G97:I97)</f>
+        <f t="shared" ref="J97:J102" si="25">AVERAGE(G97:I97)</f>
         <v>14.254612333333334</v>
       </c>
       <c r="K97" s="3">
-        <f t="shared" ref="K97:K101" si="26">I97/E97</f>
+        <f t="shared" ref="K97:K102" si="26">I97/E97</f>
         <v>1.3920216014860673E-3</v>
       </c>
       <c r="O97" s="3" t="e">
@@ -4955,29 +4960,48 @@
         <v>7</v>
       </c>
       <c r="C101">
+        <v>5000000</v>
+      </c>
+      <c r="D101">
+        <f>C101^2</f>
+        <v>25000000000000</v>
+      </c>
+      <c r="E101" s="3">
+        <f>C101 * LOG(C101, 2)</f>
+        <v>111267483.32105769</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15">
+      <c r="A102" t="s">
+        <v>15</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102">
         <v>10000000</v>
       </c>
-      <c r="D101">
+      <c r="D102">
         <f t="shared" si="22"/>
         <v>100000000000000</v>
       </c>
-      <c r="E101" s="3">
+      <c r="E102" s="3">
         <f t="shared" si="23"/>
         <v>232534966.64211538</v>
       </c>
-      <c r="I101" s="3" t="e">
+      <c r="I102" s="3" t="e">
         <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J101" t="e">
+      <c r="J102" t="e">
         <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K101" s="3" t="e">
+      <c r="K102" s="3" t="e">
         <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O101" s="3" t="e">
+      <c r="O102" s="3" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>

</xml_diff>